<commit_message>
:bug: fixed date format bug
</commit_message>
<xml_diff>
--- a/src/test/resources/卡密列表.xlsx
+++ b/src/test/resources/卡密列表.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
   <si>
     <t>卡密列表</t>
   </si>
@@ -50,9 +50,6 @@
     <t>rasefq2rzotsmx526z6g</t>
   </si>
   <si>
-    <t>2018年02月14日</t>
-  </si>
-  <si>
     <t>srcb4c9fdqzuykd6q4zl</t>
   </si>
   <si>
@@ -62,9 +59,6 @@
     <t>2ru44qut6neykb2380wt</t>
   </si>
   <si>
-    <t>2018年03月11日</t>
-  </si>
-  <si>
     <t>已使用</t>
   </si>
 </sst>
@@ -72,10 +66,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="59" formatCode="yyyy&quot;年&quot;mm&quot;月&quot;dd&quot;日 &quot;h:mm:ss"/>
-    <numFmt numFmtId="60" formatCode="yyyy&quot;年&quot;mm&quot;月&quot;dd&quot;日&quot;"/>
+    <numFmt numFmtId="59" formatCode="yyyy.m.d h:mm"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -121,12 +114,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="13"/>
+        <fgColor indexed="14"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -138,6 +131,28 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="10"/>
       </right>
@@ -151,31 +166,31 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
         <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -184,25 +199,25 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
         <color indexed="11"/>
@@ -211,31 +226,31 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -244,13 +259,28 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -260,68 +290,71 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="59" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="60" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="59" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -341,11 +374,12 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
-      <rgbColor rgb="ffffffff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1410,7 +1444,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:I6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1432,133 +1466,133 @@
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="4"/>
     </row>
     <row r="2" ht="22.55" customHeight="1">
-      <c r="A2" t="s" s="3">
+      <c r="A2" t="s" s="5">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="B2" t="s" s="5">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="C2" t="s" s="5">
         <v>3</v>
       </c>
-      <c r="D2" t="s" s="3">
+      <c r="D2" t="s" s="5">
         <v>4</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" t="s" s="3">
+      <c r="E2" s="6"/>
+      <c r="F2" t="s" s="5">
         <v>5</v>
       </c>
-      <c r="G2" t="s" s="3">
+      <c r="G2" t="s" s="5">
         <v>6</v>
       </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
     </row>
     <row r="3" ht="32.25" customHeight="1">
-      <c r="A3" t="s" s="5">
+      <c r="A3" t="s" s="7">
         <v>7</v>
       </c>
-      <c r="B3" t="s" s="6">
+      <c r="B3" t="s" s="8">
         <v>8</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="9">
         <v>100</v>
       </c>
-      <c r="D3" s="8">
-        <v>41711</v>
-      </c>
-      <c r="E3" s="9"/>
-      <c r="F3" t="s" s="10">
+      <c r="D3" s="10">
+        <v>41711.382638888892</v>
+      </c>
+      <c r="E3" s="11"/>
+      <c r="F3" t="s" s="12">
         <v>9</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="13">
         <f>C3*2</f>
         <v>200</v>
       </c>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
     </row>
     <row r="4" ht="32.05" customHeight="1">
-      <c r="A4" t="s" s="13">
+      <c r="A4" t="s" s="15">
         <v>10</v>
       </c>
-      <c r="B4" t="s" s="14">
+      <c r="B4" t="s" s="16">
         <v>11</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="17">
         <v>50</v>
       </c>
-      <c r="D4" t="s" s="10">
-        <v>12</v>
-      </c>
-      <c r="E4" s="9"/>
-      <c r="F4" t="s" s="10">
+      <c r="D4" s="10">
+        <v>41711.757638888892</v>
+      </c>
+      <c r="E4" s="11"/>
+      <c r="F4" t="s" s="12">
         <v>9</v>
       </c>
-      <c r="G4" s="16">
+      <c r="G4" s="18">
         <f>C4*2</f>
         <v>100</v>
       </c>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
     </row>
     <row r="5" ht="32.05" customHeight="1">
-      <c r="A5" t="s" s="13">
+      <c r="A5" t="s" s="15">
         <v>7</v>
       </c>
-      <c r="B5" t="s" s="14">
-        <v>13</v>
-      </c>
-      <c r="C5" s="15">
+      <c r="B5" t="s" s="16">
+        <v>12</v>
+      </c>
+      <c r="C5" s="17">
         <v>200</v>
       </c>
-      <c r="D5" s="18">
-        <v>41715</v>
-      </c>
-      <c r="E5" s="12"/>
-      <c r="F5" t="s" s="19">
+      <c r="D5" s="10">
+        <v>41407.757638888892</v>
+      </c>
+      <c r="E5" s="14"/>
+      <c r="F5" t="s" s="20">
         <v>9</v>
       </c>
-      <c r="G5" s="16">
+      <c r="G5" s="18">
         <f>C5*2</f>
         <v>400</v>
       </c>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
     </row>
     <row r="6" ht="32.05" customHeight="1">
-      <c r="A6" t="s" s="13">
+      <c r="A6" t="s" s="15">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s" s="16">
         <v>14</v>
       </c>
-      <c r="B6" t="s" s="14">
+      <c r="C6" s="17">
+        <v>100</v>
+      </c>
+      <c r="D6" s="10">
+        <v>41711.757638888892</v>
+      </c>
+      <c r="E6" s="19"/>
+      <c r="F6" t="s" s="21">
         <v>15</v>
       </c>
-      <c r="C6" s="15">
-        <v>100</v>
-      </c>
-      <c r="D6" t="s" s="10">
-        <v>16</v>
-      </c>
-      <c r="E6" s="17"/>
-      <c r="F6" t="s" s="20">
-        <v>17</v>
-      </c>
-      <c r="G6" s="16">
+      <c r="G6" s="18">
         <f>C6*2</f>
         <v>200</v>
       </c>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>